<commit_message>
EPP Variable Installments T1 scenarios
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3114-MS-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-OVERDUE-FEE-%APR-AMT-Regular-CASH-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/3114-MS-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-OVERDUE-FEE-%APR-AMT-Regular-CASH-Makerepayment1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t>#</t>
   </si>
@@ -141,15 +141,9 @@
     <t>Repayment</t>
   </si>
   <si>
-    <t>INCOME</t>
-  </si>
-  <si>
     <t>Income from interest(7)</t>
   </si>
   <si>
-    <t>L216</t>
-  </si>
-  <si>
     <t>$ 10,000</t>
   </si>
   <si>
@@ -168,22 +162,34 @@
     <t>repaymenttransactiondate</t>
   </si>
   <si>
+    <t xml:space="preserve">Head Office </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L83 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mifos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCOME </t>
+  </si>
+  <si>
+    <t>Income from penalties(9)</t>
+  </si>
+  <si>
+    <t>$ 785.8</t>
+  </si>
+  <si>
+    <t>$ 101.92</t>
+  </si>
+  <si>
+    <t>$ 7.86</t>
+  </si>
+  <si>
     <t>$ 895.58</t>
-  </si>
-  <si>
-    <t>repaymenttransactionamount</t>
-  </si>
-  <si>
-    <t>$ 101.92</t>
-  </si>
-  <si>
-    <t>$ 785.8</t>
-  </si>
-  <si>
-    <t>$ 7.86</t>
-  </si>
-  <si>
-    <t>Income from penalties(9)</t>
   </si>
 </sst>
 </file>
@@ -290,14 +296,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -321,19 +324,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,32 +648,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="17">
+      <c r="B2" s="15">
         <v>42036</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="19">
-        <v>895.58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -683,18 +673,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD14"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -718,80 +708,80 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>10000</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>785.8</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
         <v>9214.2000000000007</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>802.9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>668.41</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>101.92</v>
       </c>
-      <c r="C3" s="7">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
         <v>566.49</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>84.82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>15.89</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>7.86</v>
       </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
         <v>8.0299999999999994</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>8.0299999999999994</v>
       </c>
     </row>
@@ -803,10 +793,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +806,7 @@
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -829,7 +819,7 @@
     <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -879,587 +869,597 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7">
         <v>42005</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="8">
         <v>10000</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7">
-        <v>0</v>
-      </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7">
-        <v>0</v>
-      </c>
-      <c r="L2" s="7">
-        <v>0</v>
-      </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>31</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>42036</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>42036</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="7">
+      <c r="E3" s="10"/>
+      <c r="F3" s="6">
         <v>785.8</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="9">
         <v>9214.2000000000007</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>101.92</v>
       </c>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7">
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
         <v>7.86</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>895.58</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <v>895.58</v>
       </c>
-      <c r="M3" s="7">
-        <v>0</v>
-      </c>
-      <c r="N3" s="7">
-        <v>0</v>
-      </c>
-      <c r="O3" s="7">
-        <v>0</v>
-      </c>
-      <c r="P3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>G2*(12%/365)*B3</f>
+        <v>101.91780821917808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>28</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>42064</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6">
         <v>802.9</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <v>8411.2999999999993</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>84.82</v>
       </c>
-      <c r="I4" s="7">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
         <v>8.0299999999999994</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>895.75</v>
       </c>
-      <c r="L4" s="7">
-        <v>0</v>
-      </c>
-      <c r="M4" s="7">
-        <v>0</v>
-      </c>
-      <c r="N4" s="7">
-        <v>0</v>
-      </c>
-      <c r="O4" s="7">
-        <v>0</v>
-      </c>
-      <c r="P4" s="7">
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
         <v>895.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q14" si="0">G3*(12%/365)*B4</f>
+        <v>84.821128767123298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>31</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>42095</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
         <v>793.81</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>7617.49</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>93.91</v>
       </c>
-      <c r="I5" s="7">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
         <v>887.72</v>
       </c>
-      <c r="L5" s="7">
-        <v>0</v>
-      </c>
-      <c r="M5" s="7">
-        <v>0</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0</v>
-      </c>
-      <c r="O5" s="7">
-        <v>0</v>
-      </c>
-      <c r="P5" s="7">
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>85.726126027397257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>30</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>42125</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
         <v>812.59</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="9">
         <v>6804.9</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>75.13</v>
       </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0</v>
-      </c>
-      <c r="K6" s="7">
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
         <v>887.72</v>
       </c>
-      <c r="L6" s="7">
-        <v>0</v>
-      </c>
-      <c r="M6" s="7">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0</v>
-      </c>
-      <c r="O6" s="7">
-        <v>0</v>
-      </c>
-      <c r="P6" s="7">
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6">
         <v>887.72</v>
       </c>
-      <c r="R6" s="7"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>75.131408219178084</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>31</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>42156</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
         <v>818.37</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>5986.53</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>69.349999999999994</v>
       </c>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
         <v>887.72</v>
       </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="7">
-        <v>0</v>
-      </c>
-      <c r="O7" s="7">
-        <v>0</v>
-      </c>
-      <c r="P7" s="7">
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+      <c r="P7" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>69.354049315068494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>30</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>42186</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
         <v>828.67</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <v>5157.8599999999997</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>59.05</v>
       </c>
-      <c r="I8" s="7">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
         <v>887.72</v>
       </c>
-      <c r="L8" s="7">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7">
-        <v>0</v>
-      </c>
-      <c r="N8" s="7">
-        <v>0</v>
-      </c>
-      <c r="O8" s="7">
-        <v>0</v>
-      </c>
-      <c r="P8" s="7">
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>59.045227397260277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>31</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>42217</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
         <v>835.15</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>4322.71</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>52.57</v>
       </c>
-      <c r="I9" s="7">
-        <v>0</v>
-      </c>
-      <c r="J9" s="7">
-        <v>0</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
         <v>887.72</v>
       </c>
-      <c r="L9" s="7">
-        <v>0</v>
-      </c>
-      <c r="M9" s="7">
-        <v>0</v>
-      </c>
-      <c r="N9" s="7">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7">
-        <v>0</v>
-      </c>
-      <c r="P9" s="7">
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+      <c r="P9" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>52.567778630136985</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>31</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>42248</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
         <v>843.66</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>3479.05</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>44.06</v>
       </c>
-      <c r="I10" s="7">
-        <v>0</v>
-      </c>
-      <c r="J10" s="7">
-        <v>0</v>
-      </c>
-      <c r="K10" s="7">
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
         <v>887.72</v>
       </c>
-      <c r="L10" s="7">
-        <v>0</v>
-      </c>
-      <c r="M10" s="7">
-        <v>0</v>
-      </c>
-      <c r="N10" s="7">
-        <v>0</v>
-      </c>
-      <c r="O10" s="7">
-        <v>0</v>
-      </c>
-      <c r="P10" s="7">
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="6">
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>44.056112876712326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>30</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>42278</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6">
         <v>853.41</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>2625.64</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>34.31</v>
       </c>
-      <c r="I11" s="7">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
-        <v>0</v>
-      </c>
-      <c r="K11" s="7">
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
         <v>887.72</v>
       </c>
-      <c r="L11" s="7">
-        <v>0</v>
-      </c>
-      <c r="M11" s="7">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
-        <v>0</v>
-      </c>
-      <c r="P11" s="7">
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="6">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>34.31391780821918</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>31</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>42309</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6">
         <v>860.96</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>1764.68</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>26.76</v>
       </c>
-      <c r="I12" s="7">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
-      <c r="K12" s="7">
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
         <v>887.72</v>
       </c>
-      <c r="L12" s="7">
-        <v>0</v>
-      </c>
-      <c r="M12" s="7">
-        <v>0</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0</v>
-      </c>
-      <c r="O12" s="7">
-        <v>0</v>
-      </c>
-      <c r="P12" s="7">
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="6">
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0</v>
+      </c>
+      <c r="P12" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>26.759947397260273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>30</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>42339</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6">
         <v>870.31</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <v>894.37</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>17.41</v>
       </c>
-      <c r="I13" s="7">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
         <v>887.72</v>
       </c>
-      <c r="L13" s="7">
-        <v>0</v>
-      </c>
-      <c r="M13" s="7">
-        <v>0</v>
-      </c>
-      <c r="N13" s="7">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7">
-        <v>0</v>
-      </c>
-      <c r="P13" s="7">
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
         <v>887.72</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>17.40506301369863</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>31</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>42370</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6">
         <v>894.37</v>
       </c>
-      <c r="G14" s="7">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7">
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
         <v>9.1199999999999992</v>
       </c>
-      <c r="I14" s="7">
-        <v>0</v>
-      </c>
-      <c r="J14" s="7">
-        <v>0</v>
-      </c>
-      <c r="K14" s="7">
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
         <v>903.49</v>
       </c>
-      <c r="L14" s="7">
-        <v>0</v>
-      </c>
-      <c r="M14" s="7">
-        <v>0</v>
-      </c>
-      <c r="N14" s="7">
-        <v>0</v>
-      </c>
-      <c r="O14" s="7">
-        <v>0</v>
-      </c>
-      <c r="P14" s="7">
+      <c r="L14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="6">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
         <v>903.49</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>9.1152230136986301</v>
       </c>
     </row>
   </sheetData>
@@ -1470,25 +1470,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1524,75 +1524,72 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>3</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6">
+        <v>101</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>42036</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>895.58</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>785.8</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>101.92</v>
       </c>
-      <c r="H2" s="7">
-        <v>0</v>
-      </c>
-      <c r="I2" s="7">
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
         <v>7.86</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>9214.2000000000007</v>
       </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="11"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="6">
+        <v>97</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>42005</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>10000</v>
       </c>
-      <c r="F3" s="7">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
-      <c r="J3" s="9">
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
         <v>10000</v>
       </c>
       <c r="K3"/>
       <c r="L3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J5" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1604,37 +1601,37 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1643,13 +1640,13 @@
         <v>3640</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="15">
+        <v>43</v>
+      </c>
+      <c r="C2" s="13">
         <v>42005</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -1661,7 +1658,7 @@
         <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1669,13 +1666,13 @@
         <v>3641</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="15">
+        <v>43</v>
+      </c>
+      <c r="C3" s="13">
         <v>42005</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -1687,7 +1684,7 @@
         <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1700,155 +1697,155 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="13"/>
-    <col min="7" max="7" width="21.85546875" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="12"/>
+    <col min="7" max="7" width="21.85546875" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="A2" s="12">
+        <v>110</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="16">
         <v>42036</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="21" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>111</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="16">
+        <v>42036</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>112</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="16">
+        <v>42036</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="14">
+      <c r="H4" s="17"/>
+      <c r="I4" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>113</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="16">
         <v>42036</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="14">
-        <v>42036</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="14">
-        <v>42036</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="D5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="4"/>
+      <c r="H5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>